<commit_message>
working single account only version up to creating an allocation
</commit_message>
<xml_diff>
--- a/TradeManager/test/test_data/sellsOnly/sellsOnlySingle/SellOnlySingleAccount.xlsx
+++ b/TradeManager/test/test_data/sellsOnly/sellsOnlySingle/SellOnlySingleAccount.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,6 +458,9 @@
       <c r="D3" s="1">
         <v>98.2</v>
       </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -468,6 +471,9 @@
       </c>
       <c r="D4" s="1">
         <v>74.5</v>
+      </c>
+      <c r="E4">
+        <v>6.25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>